<commit_message>
optimization variable quick fix
</commit_message>
<xml_diff>
--- a/python3/data/params.xlsx
+++ b/python3/data/params.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\dd_winrock\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\blopti\python3\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E79E722-AD6E-484B-AAF3-2A9E942B6567}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0BB8BC-40AB-40E4-97FD-D94E32F26C0D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4608" yWindow="2280" windowWidth="17280" windowHeight="8964" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -597,17 +597,19 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+    <col min="3" max="7" width="8.5546875" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="1025" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,7 +635,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>0.4</v>
       </c>
@@ -675,12 +677,12 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1025" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>10</v>
       </c>

</xml_diff>